<commit_message>
adds parsing of Regions
</commit_message>
<xml_diff>
--- a/data/mobile music ex1.1.xlsx
+++ b/data/mobile music ex1.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="88">
   <si>
     <t>theme</t>
   </si>
@@ -158,9 +158,6 @@
     <t>disable</t>
   </si>
   <si>
-    <t>enableatstart</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -270,6 +267,21 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>enabledatstart</t>
+  </si>
+  <si>
+    <t>outfile</t>
+  </si>
+  <si>
+    <t>daoplayer-test1.json</t>
+  </si>
+  <si>
+    <t>contextfile</t>
+  </si>
+  <si>
+    <t>context-test1.json</t>
   </si>
 </sst>
 </file>
@@ -622,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,26 +648,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
         <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -663,23 +675,39 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
         <v>80</v>
-      </c>
-      <c r="B5" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>83</v>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -692,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,19 +743,19 @@
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>20</v>
@@ -736,7 +764,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>43</v>
@@ -759,30 +787,36 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
         <v>42</v>
       </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -790,16 +824,22 @@
       <c r="I3" t="s">
         <v>42</v>
       </c>
+      <c r="M3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -811,13 +851,13 @@
         <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" t="s">
         <v>57</v>
-      </c>
-      <c r="L4" t="s">
-        <v>58</v>
       </c>
       <c r="M4" t="s">
         <v>11</v>
@@ -831,25 +871,25 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5">
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" t="s">
         <v>11</v>
@@ -860,25 +900,25 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6">
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M6" t="s">
         <v>11</v>
@@ -889,13 +929,13 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F7">
         <v>10</v>
@@ -907,10 +947,10 @@
         <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M7" t="s">
         <v>11</v>
@@ -919,12 +959,12 @@
         <v>5</v>
       </c>
       <c r="O7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>22</v>
@@ -940,7 +980,7 @@
         <v>42</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M8" t="s">
         <v>24</v>
@@ -954,13 +994,13 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -977,13 +1017,13 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -992,7 +1032,7 @@
         <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M10" t="s">
         <v>24</v>
@@ -1212,7 +1252,7 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1223,10 +1263,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4">
         <v>1</v>

</xml_diff>